<commit_message>
added class for creating the matches which stores the loaded data like mappings (implemented) and obj xlsx's (unimplemented)
</commit_message>
<xml_diff>
--- a/TestSheet1.xlsx
+++ b/TestSheet1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niravs\Documents\SFCompareAndLoad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84CEA91B-E894-4040-A1BA-37D5FCED0092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F5A481-BF09-440C-986D-C1E48785C4FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{BEF77309-A07C-430D-9426-4A4BDF81F07F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{BEF77309-A07C-430D-9426-4A4BDF81F07F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2001,14 +2001,14 @@
     <t>Shipment_Order__c.r__Part__c[1].Requirement_Unknown__c</t>
   </si>
   <si>
-    <t>tecex--ruleseng</t>
+    <t>tecex--prod</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2084,12 +2084,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -2758,8 +2752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A29EAB9-F893-4E29-8E72-A16D47667C06}">
   <dimension ref="A1:F492"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8873,8 +8867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60E00B09-BA71-4F35-AAD0-572D3DDCA95E}">
   <dimension ref="A1:F492"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9263,7 +9257,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>48</v>
       </c>
@@ -9273,7 +9267,7 @@
       </c>
       <c r="E31" s="17"/>
     </row>
-    <row r="32" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>49</v>
       </c>
@@ -9283,7 +9277,7 @@
       </c>
       <c r="E32" s="17"/>
     </row>
-    <row r="33" spans="1:5" ht="240" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
         <v>50</v>
       </c>
@@ -9297,7 +9291,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="240" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>52</v>
       </c>
@@ -9307,7 +9301,7 @@
       </c>
       <c r="E34" s="17"/>
     </row>
-    <row r="35" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>53</v>
       </c>
@@ -9317,7 +9311,7 @@
       </c>
       <c r="E35" s="17"/>
     </row>
-    <row r="36" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>54</v>
       </c>
@@ -9327,7 +9321,7 @@
       </c>
       <c r="E36" s="17"/>
     </row>
-    <row r="37" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>55</v>
       </c>
@@ -9341,7 +9335,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>56</v>
       </c>
@@ -9355,7 +9349,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
         <v>58</v>
       </c>
@@ -9365,7 +9359,7 @@
       </c>
       <c r="E39" s="17"/>
     </row>
-    <row r="40" spans="1:5" ht="255" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
         <v>59</v>
       </c>
@@ -9379,7 +9373,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="300" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
         <v>61</v>
       </c>
@@ -9393,7 +9387,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="270" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
         <v>63</v>
       </c>
@@ -9407,7 +9401,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="285" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>65</v>
       </c>
@@ -9421,7 +9415,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
         <v>66</v>
       </c>
@@ -9435,7 +9429,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
         <v>68</v>
       </c>
@@ -9449,7 +9443,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
         <v>69</v>
       </c>
@@ -9463,7 +9457,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
         <v>70</v>
       </c>
@@ -9477,7 +9471,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
         <v>71</v>
       </c>
@@ -9487,7 +9481,7 @@
       </c>
       <c r="E48" s="17"/>
     </row>
-    <row r="49" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
         <v>72</v>
       </c>
@@ -9497,7 +9491,7 @@
       </c>
       <c r="E49" s="17"/>
     </row>
-    <row r="50" spans="1:5" ht="240" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
         <v>73</v>
       </c>
@@ -9511,7 +9505,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="240" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
         <v>75</v>
       </c>
@@ -9521,7 +9515,7 @@
       </c>
       <c r="E51" s="17"/>
     </row>
-    <row r="52" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
         <v>76</v>
       </c>
@@ -9531,7 +9525,7 @@
       </c>
       <c r="E52" s="17"/>
     </row>
-    <row r="53" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
         <v>77</v>
       </c>
@@ -9541,7 +9535,7 @@
       </c>
       <c r="E53" s="17"/>
     </row>
-    <row r="54" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
         <v>78</v>
       </c>
@@ -9555,7 +9549,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
         <v>79</v>
       </c>
@@ -9569,7 +9563,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
         <v>80</v>
       </c>
@@ -9579,7 +9573,7 @@
       </c>
       <c r="E56" s="17"/>
     </row>
-    <row r="57" spans="1:5" ht="255" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
         <v>81</v>
       </c>
@@ -9593,7 +9587,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="300" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
         <v>82</v>
       </c>
@@ -9607,7 +9601,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="270" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
         <v>83</v>
       </c>
@@ -9621,7 +9615,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="285" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
         <v>84</v>
       </c>
@@ -9635,7 +9629,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
         <v>85</v>
       </c>
@@ -9649,7 +9643,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
         <v>87</v>
       </c>
@@ -9663,7 +9657,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="17" t="s">
         <v>89</v>
       </c>
@@ -9677,7 +9671,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="17" t="s">
         <v>90</v>
       </c>
@@ -9691,7 +9685,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="17" t="s">
         <v>91</v>
       </c>
@@ -9701,7 +9695,7 @@
       </c>
       <c r="E65" s="17"/>
     </row>
-    <row r="66" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="17" t="s">
         <v>92</v>
       </c>
@@ -9711,7 +9705,7 @@
       </c>
       <c r="E66" s="17"/>
     </row>
-    <row r="67" spans="1:5" ht="240" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="17" t="s">
         <v>93</v>
       </c>
@@ -9725,7 +9719,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="240" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
         <v>95</v>
       </c>
@@ -9735,7 +9729,7 @@
       </c>
       <c r="E68" s="17"/>
     </row>
-    <row r="69" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="17" t="s">
         <v>96</v>
       </c>
@@ -9745,7 +9739,7 @@
       </c>
       <c r="E69" s="17"/>
     </row>
-    <row r="70" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="17" t="s">
         <v>97</v>
       </c>
@@ -9755,7 +9749,7 @@
       </c>
       <c r="E70" s="17"/>
     </row>
-    <row r="71" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="17" t="s">
         <v>98</v>
       </c>
@@ -9769,7 +9763,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="17" t="s">
         <v>99</v>
       </c>
@@ -9779,7 +9773,7 @@
       </c>
       <c r="E72" s="17"/>
     </row>
-    <row r="73" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="17" t="s">
         <v>100</v>
       </c>
@@ -9789,7 +9783,7 @@
       </c>
       <c r="E73" s="17"/>
     </row>
-    <row r="74" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="17" t="s">
         <v>101</v>
       </c>
@@ -9803,7 +9797,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="17" t="s">
         <v>103</v>
       </c>
@@ -9813,7 +9807,7 @@
       </c>
       <c r="E75" s="17"/>
     </row>
-    <row r="76" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="17" t="s">
         <v>104</v>
       </c>
@@ -9827,7 +9821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="17" t="s">
         <v>105</v>
       </c>
@@ -9841,7 +9835,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="17" t="s">
         <v>106</v>
       </c>
@@ -9851,7 +9845,7 @@
       </c>
       <c r="E78" s="17"/>
     </row>
-    <row r="79" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="17" t="s">
         <v>107</v>
       </c>
@@ -9861,7 +9855,7 @@
       </c>
       <c r="E79" s="17"/>
     </row>
-    <row r="80" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="17" t="s">
         <v>108</v>
       </c>
@@ -9875,7 +9869,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="17" t="s">
         <v>110</v>
       </c>
@@ -9889,7 +9883,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="17" t="s">
         <v>111</v>
       </c>
@@ -9899,7 +9893,7 @@
       </c>
       <c r="E82" s="17"/>
     </row>
-    <row r="83" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="17" t="s">
         <v>112</v>
       </c>
@@ -9913,7 +9907,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="17" t="s">
         <v>113</v>
       </c>
@@ -9927,7 +9921,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="17" t="s">
         <v>115</v>
       </c>
@@ -9937,7 +9931,7 @@
       </c>
       <c r="E85" s="17"/>
     </row>
-    <row r="86" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="17" t="s">
         <v>116</v>
       </c>
@@ -9947,7 +9941,7 @@
       </c>
       <c r="E86" s="17"/>
     </row>
-    <row r="87" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="17" t="s">
         <v>117</v>
       </c>
@@ -9957,7 +9951,7 @@
       </c>
       <c r="E87" s="17"/>
     </row>
-    <row r="88" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="17" t="s">
         <v>118</v>
       </c>
@@ -9971,7 +9965,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="17" t="s">
         <v>120</v>
       </c>
@@ -9981,7 +9975,7 @@
       </c>
       <c r="E89" s="17"/>
     </row>
-    <row r="90" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="17" t="s">
         <v>121</v>
       </c>
@@ -9991,7 +9985,7 @@
       </c>
       <c r="E90" s="17"/>
     </row>
-    <row r="91" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="17" t="s">
         <v>122</v>
       </c>
@@ -10001,7 +9995,7 @@
       </c>
       <c r="E91" s="17"/>
     </row>
-    <row r="92" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="17" t="s">
         <v>123</v>
       </c>
@@ -10011,7 +10005,7 @@
       </c>
       <c r="E92" s="17"/>
     </row>
-    <row r="93" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="17" t="s">
         <v>124</v>
       </c>
@@ -10021,7 +10015,7 @@
       </c>
       <c r="E93" s="17"/>
     </row>
-    <row r="94" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="17" t="s">
         <v>125</v>
       </c>
@@ -10031,7 +10025,7 @@
       </c>
       <c r="E94" s="17"/>
     </row>
-    <row r="95" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="17" t="s">
         <v>126</v>
       </c>
@@ -10041,7 +10035,7 @@
       </c>
       <c r="E95" s="17"/>
     </row>
-    <row r="96" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="17" t="s">
         <v>127</v>
       </c>
@@ -10055,7 +10049,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="17" t="s">
         <v>129</v>
       </c>
@@ -10069,7 +10063,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="17" t="s">
         <v>131</v>
       </c>
@@ -10083,7 +10077,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="17" t="s">
         <v>133</v>
       </c>
@@ -10097,7 +10091,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="17" t="s">
         <v>134</v>
       </c>
@@ -10111,7 +10105,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="17" t="s">
         <v>136</v>
       </c>
@@ -10125,7 +10119,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="17" t="s">
         <v>138</v>
       </c>
@@ -10139,7 +10133,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="17" t="s">
         <v>140</v>
       </c>
@@ -10153,7 +10147,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="17" t="s">
         <v>141</v>
       </c>
@@ -10167,7 +10161,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="17" t="s">
         <v>143</v>
       </c>
@@ -10181,7 +10175,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="17" t="s">
         <v>145</v>
       </c>
@@ -10195,7 +10189,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="17" t="s">
         <v>147</v>
       </c>
@@ -10209,7 +10203,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="17" t="s">
         <v>148</v>
       </c>
@@ -10223,7 +10217,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="17" t="s">
         <v>150</v>
       </c>
@@ -10237,7 +10231,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="17" t="s">
         <v>152</v>
       </c>
@@ -10251,7 +10245,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="17" t="s">
         <v>154</v>
       </c>
@@ -10265,7 +10259,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="17" t="s">
         <v>155</v>
       </c>
@@ -10279,7 +10273,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="17" t="s">
         <v>157</v>
       </c>
@@ -10293,7 +10287,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="17" t="s">
         <v>159</v>
       </c>
@@ -10307,7 +10301,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="17" t="s">
         <v>161</v>
       </c>
@@ -10321,7 +10315,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="17" t="s">
         <v>162</v>
       </c>
@@ -10335,7 +10329,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="17" t="s">
         <v>164</v>
       </c>
@@ -10349,7 +10343,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="17" t="s">
         <v>166</v>
       </c>
@@ -10363,7 +10357,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="17" t="s">
         <v>168</v>
       </c>
@@ -10377,7 +10371,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="17" t="s">
         <v>169</v>
       </c>
@@ -10391,7 +10385,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="17" t="s">
         <v>171</v>
       </c>
@@ -10405,7 +10399,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="17" t="s">
         <v>173</v>
       </c>
@@ -10419,7 +10413,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" s="17" t="s">
         <v>175</v>
       </c>
@@ -10433,7 +10427,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="17" t="s">
         <v>176</v>
       </c>
@@ -10447,7 +10441,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="17" t="s">
         <v>178</v>
       </c>
@@ -10461,7 +10455,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="17" t="s">
         <v>180</v>
       </c>
@@ -10475,7 +10469,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" s="17" t="s">
         <v>182</v>
       </c>
@@ -10489,7 +10483,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="17" t="s">
         <v>183</v>
       </c>
@@ -10503,7 +10497,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A129" s="17" t="s">
         <v>185</v>
       </c>
@@ -10517,7 +10511,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" s="17" t="s">
         <v>187</v>
       </c>
@@ -10531,7 +10525,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A131" s="17" t="s">
         <v>189</v>
       </c>
@@ -10545,7 +10539,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="17" t="s">
         <v>190</v>
       </c>
@@ -10559,7 +10553,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="17" t="s">
         <v>192</v>
       </c>
@@ -10573,7 +10567,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="17" t="s">
         <v>194</v>
       </c>
@@ -10587,7 +10581,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="17" t="s">
         <v>196</v>
       </c>
@@ -10601,7 +10595,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" s="17" t="s">
         <v>197</v>
       </c>
@@ -10615,7 +10609,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A137" s="17" t="s">
         <v>199</v>
       </c>
@@ -10629,7 +10623,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" s="17" t="s">
         <v>201</v>
       </c>
@@ -10643,7 +10637,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="17" t="s">
         <v>203</v>
       </c>
@@ -10657,7 +10651,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="17" t="s">
         <v>204</v>
       </c>
@@ -10671,7 +10665,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A141" s="17" t="s">
         <v>206</v>
       </c>
@@ -10685,7 +10679,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A142" s="17" t="s">
         <v>208</v>
       </c>
@@ -10699,7 +10693,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="17" t="s">
         <v>210</v>
       </c>
@@ -10713,7 +10707,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="17" t="s">
         <v>211</v>
       </c>
@@ -10727,7 +10721,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="17" t="s">
         <v>212</v>
       </c>
@@ -10741,7 +10735,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="17" t="s">
         <v>214</v>
       </c>
@@ -10755,7 +10749,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A147" s="17" t="s">
         <v>216</v>
       </c>
@@ -10769,7 +10763,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="17" t="s">
         <v>218</v>
       </c>
@@ -10779,7 +10773,7 @@
       </c>
       <c r="E148" s="17"/>
     </row>
-    <row r="149" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="17" t="s">
         <v>219</v>
       </c>
@@ -10793,7 +10787,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" s="17" t="s">
         <v>221</v>
       </c>
@@ -10803,7 +10797,7 @@
       </c>
       <c r="E150" s="17"/>
     </row>
-    <row r="151" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" s="17" t="s">
         <v>222</v>
       </c>
@@ -10813,7 +10807,7 @@
       </c>
       <c r="E151" s="17"/>
     </row>
-    <row r="152" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="17" t="s">
         <v>223</v>
       </c>
@@ -10827,7 +10821,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" s="17" t="s">
         <v>225</v>
       </c>
@@ -10841,7 +10835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="17" t="s">
         <v>226</v>
       </c>
@@ -10851,7 +10845,7 @@
       </c>
       <c r="E154" s="17"/>
     </row>
-    <row r="155" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="17" t="s">
         <v>227</v>
       </c>
@@ -10865,7 +10859,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="17" t="s">
         <v>229</v>
       </c>
@@ -10875,7 +10869,7 @@
       </c>
       <c r="E156" s="17"/>
     </row>
-    <row r="157" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="17" t="s">
         <v>230</v>
       </c>
@@ -10885,7 +10879,7 @@
       </c>
       <c r="E157" s="17"/>
     </row>
-    <row r="158" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="17" t="s">
         <v>231</v>
       </c>
@@ -10899,7 +10893,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="17" t="s">
         <v>232</v>
       </c>
@@ -10913,7 +10907,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" s="17" t="s">
         <v>234</v>
       </c>
@@ -10927,7 +10921,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" s="17" t="s">
         <v>236</v>
       </c>
@@ -10941,7 +10935,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="17" t="s">
         <v>237</v>
       </c>
@@ -10951,7 +10945,7 @@
       </c>
       <c r="E162" s="17"/>
     </row>
-    <row r="163" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="17" t="s">
         <v>238</v>
       </c>
@@ -10965,7 +10959,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="164" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="17" t="s">
         <v>240</v>
       </c>
@@ -10975,7 +10969,7 @@
       </c>
       <c r="E164" s="17"/>
     </row>
-    <row r="165" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" s="17" t="s">
         <v>241</v>
       </c>
@@ -10985,7 +10979,7 @@
       </c>
       <c r="E165" s="17"/>
     </row>
-    <row r="166" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="17" t="s">
         <v>242</v>
       </c>
@@ -10999,7 +10993,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="167" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A167" s="17" t="s">
         <v>244</v>
       </c>
@@ -11013,7 +11007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" s="17" t="s">
         <v>245</v>
       </c>
@@ -11023,7 +11017,7 @@
       </c>
       <c r="E168" s="17"/>
     </row>
-    <row r="169" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="17" t="s">
         <v>246</v>
       </c>
@@ -11037,7 +11031,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="170" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="17" t="s">
         <v>247</v>
       </c>
@@ -11047,7 +11041,7 @@
       </c>
       <c r="E170" s="17"/>
     </row>
-    <row r="171" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="17" t="s">
         <v>248</v>
       </c>
@@ -11057,7 +11051,7 @@
       </c>
       <c r="E171" s="17"/>
     </row>
-    <row r="172" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="17" t="s">
         <v>249</v>
       </c>
@@ -11071,7 +11065,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="173" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A173" s="17" t="s">
         <v>250</v>
       </c>
@@ -11085,7 +11079,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="174" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A174" s="17" t="s">
         <v>252</v>
       </c>
@@ -11099,7 +11093,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="175" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A175" s="17" t="s">
         <v>254</v>
       </c>
@@ -11113,7 +11107,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="176" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="17" t="s">
         <v>255</v>
       </c>
@@ -11123,7 +11117,7 @@
       </c>
       <c r="E176" s="17"/>
     </row>
-    <row r="177" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="17" t="s">
         <v>256</v>
       </c>
@@ -11137,7 +11131,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="178" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A178" s="17" t="s">
         <v>257</v>
       </c>
@@ -11147,7 +11141,7 @@
       </c>
       <c r="E178" s="17"/>
     </row>
-    <row r="179" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="17" t="s">
         <v>258</v>
       </c>
@@ -11157,7 +11151,7 @@
       </c>
       <c r="E179" s="17"/>
     </row>
-    <row r="180" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A180" s="17" t="s">
         <v>259</v>
       </c>
@@ -11171,7 +11165,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="181" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A181" s="17" t="s">
         <v>261</v>
       </c>
@@ -11185,7 +11179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" s="17" t="s">
         <v>262</v>
       </c>
@@ -11195,7 +11189,7 @@
       </c>
       <c r="E182" s="17"/>
     </row>
-    <row r="183" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A183" s="17" t="s">
         <v>263</v>
       </c>
@@ -11209,7 +11203,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="184" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" s="17" t="s">
         <v>264</v>
       </c>
@@ -11219,7 +11213,7 @@
       </c>
       <c r="E184" s="17"/>
     </row>
-    <row r="185" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A185" s="17" t="s">
         <v>265</v>
       </c>
@@ -11229,7 +11223,7 @@
       </c>
       <c r="E185" s="17"/>
     </row>
-    <row r="186" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A186" s="17" t="s">
         <v>266</v>
       </c>
@@ -11243,7 +11237,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="187" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A187" s="17" t="s">
         <v>267</v>
       </c>
@@ -11257,7 +11251,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="188" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A188" s="17" t="s">
         <v>269</v>
       </c>
@@ -11271,7 +11265,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="189" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A189" s="17" t="s">
         <v>271</v>
       </c>
@@ -11285,7 +11279,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="190" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A190" s="17" t="s">
         <v>272</v>
       </c>
@@ -11295,7 +11289,7 @@
       </c>
       <c r="E190" s="17"/>
     </row>
-    <row r="191" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A191" s="17" t="s">
         <v>273</v>
       </c>
@@ -11309,7 +11303,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="192" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A192" s="17" t="s">
         <v>274</v>
       </c>
@@ -11319,7 +11313,7 @@
       </c>
       <c r="E192" s="17"/>
     </row>
-    <row r="193" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A193" s="17" t="s">
         <v>275</v>
       </c>
@@ -11329,7 +11323,7 @@
       </c>
       <c r="E193" s="17"/>
     </row>
-    <row r="194" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A194" s="17" t="s">
         <v>276</v>
       </c>
@@ -11343,7 +11337,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="195" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A195" s="17" t="s">
         <v>278</v>
       </c>
@@ -11357,7 +11351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A196" s="17" t="s">
         <v>279</v>
       </c>
@@ -11367,7 +11361,7 @@
       </c>
       <c r="E196" s="17"/>
     </row>
-    <row r="197" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A197" s="17" t="s">
         <v>280</v>
       </c>
@@ -11381,7 +11375,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="198" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A198" s="17" t="s">
         <v>281</v>
       </c>
@@ -11391,7 +11385,7 @@
       </c>
       <c r="E198" s="17"/>
     </row>
-    <row r="199" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A199" s="17" t="s">
         <v>282</v>
       </c>
@@ -11405,7 +11399,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="200" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A200" s="17" t="s">
         <v>284</v>
       </c>
@@ -11419,7 +11413,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="201" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A201" s="17" t="s">
         <v>285</v>
       </c>
@@ -11433,7 +11427,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="202" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A202" s="17" t="s">
         <v>287</v>
       </c>
@@ -11447,7 +11441,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="203" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A203" s="17" t="s">
         <v>288</v>
       </c>
@@ -11461,7 +11455,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="204" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A204" s="17" t="s">
         <v>289</v>
       </c>
@@ -11471,7 +11465,7 @@
       </c>
       <c r="E204" s="17"/>
     </row>
-    <row r="205" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A205" s="17" t="s">
         <v>290</v>
       </c>
@@ -11485,7 +11479,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="206" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A206" s="17" t="s">
         <v>292</v>
       </c>
@@ -11495,7 +11489,7 @@
       </c>
       <c r="E206" s="17"/>
     </row>
-    <row r="207" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A207" s="17" t="s">
         <v>293</v>
       </c>
@@ -11505,7 +11499,7 @@
       </c>
       <c r="E207" s="17"/>
     </row>
-    <row r="208" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A208" s="17" t="s">
         <v>294</v>
       </c>
@@ -11519,7 +11513,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="209" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A209" s="17" t="s">
         <v>296</v>
       </c>
@@ -11533,7 +11527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A210" s="17" t="s">
         <v>297</v>
       </c>
@@ -11543,7 +11537,7 @@
       </c>
       <c r="E210" s="17"/>
     </row>
-    <row r="211" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A211" s="17" t="s">
         <v>298</v>
       </c>
@@ -11557,7 +11551,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="212" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A212" s="17" t="s">
         <v>299</v>
       </c>
@@ -11567,7 +11561,7 @@
       </c>
       <c r="E212" s="17"/>
     </row>
-    <row r="213" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A213" s="17" t="s">
         <v>300</v>
       </c>
@@ -11581,7 +11575,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="214" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A214" s="17" t="s">
         <v>301</v>
       </c>
@@ -11595,7 +11589,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="215" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A215" s="17" t="s">
         <v>302</v>
       </c>
@@ -11609,7 +11603,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="216" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A216" s="17" t="s">
         <v>304</v>
       </c>
@@ -11623,7 +11617,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="217" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A217" s="17" t="s">
         <v>305</v>
       </c>
@@ -11637,7 +11631,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="218" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A218" s="17" t="s">
         <v>306</v>
       </c>
@@ -11651,7 +11645,7 @@
         <v>48752</v>
       </c>
     </row>
-    <row r="219" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A219" s="17" t="s">
         <v>307</v>
       </c>
@@ -11665,7 +11659,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="220" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A220" s="17" t="s">
         <v>308</v>
       </c>
@@ -11675,7 +11669,7 @@
       </c>
       <c r="E220" s="17"/>
     </row>
-    <row r="221" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A221" s="17" t="s">
         <v>309</v>
       </c>
@@ -11685,7 +11679,7 @@
       </c>
       <c r="E221" s="17"/>
     </row>
-    <row r="222" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A222" s="17" t="s">
         <v>310</v>
       </c>
@@ -11699,7 +11693,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="223" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A223" s="17" t="s">
         <v>312</v>
       </c>
@@ -11713,7 +11707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A224" s="17" t="s">
         <v>313</v>
       </c>
@@ -11727,7 +11721,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="225" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A225" s="17" t="s">
         <v>315</v>
       </c>
@@ -11741,7 +11735,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="226" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A226" s="17" t="s">
         <v>316</v>
       </c>
@@ -11751,7 +11745,7 @@
       </c>
       <c r="E226" s="17"/>
     </row>
-    <row r="227" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="17" t="s">
         <v>317</v>
       </c>
@@ -11765,7 +11759,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="228" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A228" s="17" t="s">
         <v>319</v>
       </c>
@@ -11779,7 +11773,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="229" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A229" s="17" t="s">
         <v>320</v>
       </c>
@@ -11793,7 +11787,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="230" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A230" s="17" t="s">
         <v>322</v>
       </c>
@@ -11807,7 +11801,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="231" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A231" s="17" t="s">
         <v>323</v>
       </c>
@@ -11821,7 +11815,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="232" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A232" s="17" t="s">
         <v>324</v>
       </c>
@@ -11835,7 +11829,7 @@
         <v>48388</v>
       </c>
     </row>
-    <row r="233" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A233" s="17" t="s">
         <v>325</v>
       </c>
@@ -11849,7 +11843,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="234" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A234" s="17" t="s">
         <v>326</v>
       </c>
@@ -11859,7 +11853,7 @@
       </c>
       <c r="E234" s="17"/>
     </row>
-    <row r="235" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A235" s="17" t="s">
         <v>327</v>
       </c>
@@ -11869,7 +11863,7 @@
       </c>
       <c r="E235" s="17"/>
     </row>
-    <row r="236" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A236" s="17" t="s">
         <v>328</v>
       </c>
@@ -11883,7 +11877,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="237" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A237" s="17" t="s">
         <v>330</v>
       </c>
@@ -11897,7 +11891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A238" s="17" t="s">
         <v>331</v>
       </c>
@@ -11911,7 +11905,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="239" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A239" s="17" t="s">
         <v>332</v>
       </c>
@@ -11925,7 +11919,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="240" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A240" s="17" t="s">
         <v>333</v>
       </c>
@@ -11935,7 +11929,7 @@
       </c>
       <c r="E240" s="17"/>
     </row>
-    <row r="241" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A241" s="17" t="s">
         <v>334</v>
       </c>
@@ -11949,7 +11943,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="242" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A242" s="17" t="s">
         <v>335</v>
       </c>
@@ -11963,7 +11957,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="243" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A243" s="17" t="s">
         <v>336</v>
       </c>
@@ -11977,7 +11971,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="244" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A244" s="17" t="s">
         <v>338</v>
       </c>
@@ -11991,7 +11985,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="245" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A245" s="17" t="s">
         <v>339</v>
       </c>
@@ -12005,7 +11999,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="246" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A246" s="17" t="s">
         <v>340</v>
       </c>
@@ -12015,7 +12009,7 @@
       </c>
       <c r="E246" s="17"/>
     </row>
-    <row r="247" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A247" s="17" t="s">
         <v>341</v>
       </c>
@@ -12029,7 +12023,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="248" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A248" s="17" t="s">
         <v>342</v>
       </c>
@@ -12039,7 +12033,7 @@
       </c>
       <c r="E248" s="17"/>
     </row>
-    <row r="249" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A249" s="17" t="s">
         <v>343</v>
       </c>
@@ -12049,7 +12043,7 @@
       </c>
       <c r="E249" s="17"/>
     </row>
-    <row r="250" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A250" s="17" t="s">
         <v>344</v>
       </c>
@@ -12063,7 +12057,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="251" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A251" s="17" t="s">
         <v>346</v>
       </c>
@@ -12077,7 +12071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A252" s="17" t="s">
         <v>347</v>
       </c>
@@ -12087,7 +12081,7 @@
       </c>
       <c r="E252" s="17"/>
     </row>
-    <row r="253" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A253" s="17" t="s">
         <v>348</v>
       </c>
@@ -12101,7 +12095,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="254" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A254" s="17" t="s">
         <v>349</v>
       </c>
@@ -12111,7 +12105,7 @@
       </c>
       <c r="E254" s="17"/>
     </row>
-    <row r="255" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A255" s="17" t="s">
         <v>350</v>
       </c>
@@ -12121,7 +12115,7 @@
       </c>
       <c r="E255" s="17"/>
     </row>
-    <row r="256" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A256" s="17" t="s">
         <v>351</v>
       </c>
@@ -12135,7 +12129,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="257" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A257" s="17" t="s">
         <v>352</v>
       </c>
@@ -12149,7 +12143,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="258" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A258" s="17" t="s">
         <v>354</v>
       </c>
@@ -12163,7 +12157,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="259" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A259" s="17" t="s">
         <v>355</v>
       </c>
@@ -12177,7 +12171,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="260" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A260" s="17" t="s">
         <v>357</v>
       </c>
@@ -12191,7 +12185,7 @@
         <v>44733</v>
       </c>
     </row>
-    <row r="261" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A261" s="17" t="s">
         <v>358</v>
       </c>
@@ -12205,7 +12199,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="262" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A262" s="17" t="s">
         <v>359</v>
       </c>
@@ -12215,7 +12209,7 @@
       </c>
       <c r="E262" s="17"/>
     </row>
-    <row r="263" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A263" s="17" t="s">
         <v>360</v>
       </c>
@@ -12225,7 +12219,7 @@
       </c>
       <c r="E263" s="17"/>
     </row>
-    <row r="264" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A264" s="17" t="s">
         <v>361</v>
       </c>
@@ -12239,7 +12233,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="265" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A265" s="17" t="s">
         <v>363</v>
       </c>
@@ -12253,7 +12247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A266" s="17" t="s">
         <v>364</v>
       </c>
@@ -12263,7 +12257,7 @@
       </c>
       <c r="E266" s="17"/>
     </row>
-    <row r="267" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A267" s="17" t="s">
         <v>365</v>
       </c>
@@ -12277,7 +12271,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="268" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A268" s="17" t="s">
         <v>367</v>
       </c>
@@ -12287,7 +12281,7 @@
       </c>
       <c r="E268" s="17"/>
     </row>
-    <row r="269" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A269" s="17" t="s">
         <v>368</v>
       </c>
@@ -12297,7 +12291,7 @@
       </c>
       <c r="E269" s="17"/>
     </row>
-    <row r="270" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A270" s="17" t="s">
         <v>369</v>
       </c>
@@ -12311,7 +12305,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="271" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A271" s="17" t="s">
         <v>370</v>
       </c>
@@ -12325,7 +12319,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="272" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A272" s="17" t="s">
         <v>372</v>
       </c>
@@ -12339,7 +12333,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="273" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A273" s="17" t="s">
         <v>373</v>
       </c>
@@ -12353,7 +12347,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="274" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A274" s="17" t="s">
         <v>374</v>
       </c>
@@ -12367,7 +12361,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="275" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A275" s="17" t="s">
         <v>375</v>
       </c>
@@ -12381,7 +12375,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="276" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A276" s="17" t="s">
         <v>376</v>
       </c>
@@ -12391,7 +12385,7 @@
       </c>
       <c r="E276" s="17"/>
     </row>
-    <row r="277" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A277" s="17" t="s">
         <v>377</v>
       </c>
@@ -12401,7 +12395,7 @@
       </c>
       <c r="E277" s="17"/>
     </row>
-    <row r="278" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A278" s="17" t="s">
         <v>378</v>
       </c>
@@ -12415,7 +12409,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="279" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A279" s="17" t="s">
         <v>379</v>
       </c>
@@ -12429,7 +12423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A280" s="17" t="s">
         <v>380</v>
       </c>
@@ -12439,7 +12433,7 @@
       </c>
       <c r="E280" s="17"/>
     </row>
-    <row r="281" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A281" s="17" t="s">
         <v>381</v>
       </c>
@@ -12453,7 +12447,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="282" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A282" s="17" t="s">
         <v>382</v>
       </c>
@@ -12463,7 +12457,7 @@
       </c>
       <c r="E282" s="17"/>
     </row>
-    <row r="283" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A283" s="17" t="s">
         <v>383</v>
       </c>
@@ -12473,7 +12467,7 @@
       </c>
       <c r="E283" s="17"/>
     </row>
-    <row r="284" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A284" s="17" t="s">
         <v>384</v>
       </c>
@@ -12487,7 +12481,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="285" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A285" s="17" t="s">
         <v>385</v>
       </c>
@@ -12501,7 +12495,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="286" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A286" s="17" t="s">
         <v>387</v>
       </c>
@@ -12515,7 +12509,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="287" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A287" s="17" t="s">
         <v>388</v>
       </c>
@@ -12529,7 +12523,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="288" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A288" s="17" t="s">
         <v>389</v>
       </c>
@@ -12539,7 +12533,7 @@
       </c>
       <c r="E288" s="17"/>
     </row>
-    <row r="289" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A289" s="17" t="s">
         <v>390</v>
       </c>
@@ -12553,7 +12547,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="290" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A290" s="17" t="s">
         <v>391</v>
       </c>
@@ -12563,7 +12557,7 @@
       </c>
       <c r="E290" s="17"/>
     </row>
-    <row r="291" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A291" s="17" t="s">
         <v>392</v>
       </c>
@@ -12573,7 +12567,7 @@
       </c>
       <c r="E291" s="17"/>
     </row>
-    <row r="292" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A292" s="17" t="s">
         <v>393</v>
       </c>
@@ -12587,7 +12581,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="293" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A293" s="17" t="s">
         <v>394</v>
       </c>
@@ -12601,7 +12595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A294" s="17" t="s">
         <v>395</v>
       </c>
@@ -12611,7 +12605,7 @@
       </c>
       <c r="E294" s="17"/>
     </row>
-    <row r="295" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A295" s="17" t="s">
         <v>396</v>
       </c>
@@ -12625,7 +12619,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="296" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A296" s="17" t="s">
         <v>397</v>
       </c>
@@ -12635,7 +12629,7 @@
       </c>
       <c r="E296" s="17"/>
     </row>
-    <row r="297" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A297" s="17" t="s">
         <v>398</v>
       </c>
@@ -12645,7 +12639,7 @@
       </c>
       <c r="E297" s="17"/>
     </row>
-    <row r="298" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A298" s="17" t="s">
         <v>399</v>
       </c>
@@ -12659,7 +12653,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="299" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A299" s="17" t="s">
         <v>400</v>
       </c>
@@ -12673,7 +12667,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="300" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A300" s="17" t="s">
         <v>402</v>
       </c>
@@ -12687,7 +12681,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="301" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A301" s="17" t="s">
         <v>403</v>
       </c>
@@ -12701,7 +12695,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="302" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A302" s="17" t="s">
         <v>404</v>
       </c>
@@ -12711,7 +12705,7 @@
       </c>
       <c r="E302" s="17"/>
     </row>
-    <row r="303" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A303" s="17" t="s">
         <v>405</v>
       </c>
@@ -12725,7 +12719,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="304" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A304" s="17" t="s">
         <v>406</v>
       </c>
@@ -12735,7 +12729,7 @@
       </c>
       <c r="E304" s="17"/>
     </row>
-    <row r="305" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A305" s="17" t="s">
         <v>407</v>
       </c>
@@ -12745,7 +12739,7 @@
       </c>
       <c r="E305" s="17"/>
     </row>
-    <row r="306" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A306" s="17" t="s">
         <v>408</v>
       </c>
@@ -12759,7 +12753,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="307" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A307" s="17" t="s">
         <v>409</v>
       </c>
@@ -12773,7 +12767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A308" s="17" t="s">
         <v>410</v>
       </c>
@@ -12783,7 +12777,7 @@
       </c>
       <c r="E308" s="17"/>
     </row>
-    <row r="309" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A309" s="17" t="s">
         <v>411</v>
       </c>
@@ -12797,7 +12791,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="310" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A310" s="17" t="s">
         <v>412</v>
       </c>
@@ -12807,7 +12801,7 @@
       </c>
       <c r="E310" s="17"/>
     </row>
-    <row r="311" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A311" s="17" t="s">
         <v>413</v>
       </c>
@@ -12817,7 +12811,7 @@
       </c>
       <c r="E311" s="17"/>
     </row>
-    <row r="312" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="17" t="s">
         <v>414</v>
       </c>
@@ -12831,7 +12825,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="313" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="17" t="s">
         <v>416</v>
       </c>
@@ -12841,7 +12835,7 @@
       </c>
       <c r="E313" s="17"/>
     </row>
-    <row r="314" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="17" t="s">
         <v>417</v>
       </c>
@@ -12855,7 +12849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="17" t="s">
         <v>418</v>
       </c>
@@ -12869,7 +12863,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="316" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="17" t="s">
         <v>419</v>
       </c>
@@ -12879,7 +12873,7 @@
       </c>
       <c r="E316" s="17"/>
     </row>
-    <row r="317" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="17" t="s">
         <v>420</v>
       </c>
@@ -12889,7 +12883,7 @@
       </c>
       <c r="E317" s="17"/>
     </row>
-    <row r="318" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" s="17" t="s">
         <v>421</v>
       </c>
@@ -12903,7 +12897,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="319" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="17" t="s">
         <v>423</v>
       </c>
@@ -12917,7 +12911,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="320" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="17" t="s">
         <v>424</v>
       </c>
@@ -12927,7 +12921,7 @@
       </c>
       <c r="E320" s="17"/>
     </row>
-    <row r="321" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" s="17" t="s">
         <v>425</v>
       </c>
@@ -12941,7 +12935,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="322" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A322" s="17" t="s">
         <v>426</v>
       </c>
@@ -12955,7 +12949,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="323" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" s="17" t="s">
         <v>428</v>
       </c>
@@ -12965,7 +12959,7 @@
       </c>
       <c r="E323" s="17"/>
     </row>
-    <row r="324" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" s="17" t="s">
         <v>429</v>
       </c>
@@ -12975,7 +12969,7 @@
       </c>
       <c r="E324" s="17"/>
     </row>
-    <row r="325" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" s="17" t="s">
         <v>430</v>
       </c>
@@ -12985,7 +12979,7 @@
       </c>
       <c r="E325" s="17"/>
     </row>
-    <row r="326" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" s="17" t="s">
         <v>431</v>
       </c>
@@ -12995,7 +12989,7 @@
       </c>
       <c r="E326" s="17"/>
     </row>
-    <row r="327" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" s="17" t="s">
         <v>432</v>
       </c>
@@ -13005,7 +12999,7 @@
       </c>
       <c r="E327" s="17"/>
     </row>
-    <row r="328" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" s="17" t="s">
         <v>433</v>
       </c>
@@ -13015,7 +13009,7 @@
       </c>
       <c r="E328" s="17"/>
     </row>
-    <row r="329" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" s="17" t="s">
         <v>434</v>
       </c>
@@ -13025,7 +13019,7 @@
       </c>
       <c r="E329" s="17"/>
     </row>
-    <row r="330" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A330" s="17" t="s">
         <v>435</v>
       </c>
@@ -13035,7 +13029,7 @@
       </c>
       <c r="E330" s="17"/>
     </row>
-    <row r="331" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" s="17" t="s">
         <v>436</v>
       </c>
@@ -13045,7 +13039,7 @@
       </c>
       <c r="E331" s="17"/>
     </row>
-    <row r="332" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" s="17" t="s">
         <v>437</v>
       </c>
@@ -13055,7 +13049,7 @@
       </c>
       <c r="E332" s="17"/>
     </row>
-    <row r="333" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" s="17" t="s">
         <v>438</v>
       </c>
@@ -13065,7 +13059,7 @@
       </c>
       <c r="E333" s="17"/>
     </row>
-    <row r="334" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A334" s="17" t="s">
         <v>439</v>
       </c>
@@ -13079,7 +13073,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="335" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A335" s="17" t="s">
         <v>441</v>
       </c>
@@ -13093,7 +13087,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="336" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A336" s="17" t="s">
         <v>443</v>
       </c>
@@ -13107,7 +13101,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="337" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A337" s="17" t="s">
         <v>445</v>
       </c>
@@ -13121,7 +13115,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="338" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A338" s="17" t="s">
         <v>446</v>
       </c>
@@ -13135,7 +13129,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="339" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A339" s="17" t="s">
         <v>448</v>
       </c>
@@ -13149,7 +13143,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="340" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A340" s="17" t="s">
         <v>450</v>
       </c>
@@ -13163,7 +13157,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="341" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A341" s="17" t="s">
         <v>452</v>
       </c>
@@ -13177,7 +13171,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="342" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A342" s="17" t="s">
         <v>453</v>
       </c>
@@ -13191,7 +13185,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="343" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A343" s="17" t="s">
         <v>455</v>
       </c>
@@ -13205,7 +13199,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="344" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A344" s="17" t="s">
         <v>457</v>
       </c>
@@ -13219,7 +13213,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="345" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A345" s="17" t="s">
         <v>459</v>
       </c>
@@ -13233,7 +13227,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="346" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A346" s="17" t="s">
         <v>460</v>
       </c>
@@ -13247,7 +13241,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="347" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A347" s="17" t="s">
         <v>462</v>
       </c>
@@ -13261,7 +13255,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="348" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A348" s="17" t="s">
         <v>464</v>
       </c>
@@ -13275,7 +13269,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="349" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A349" s="17" t="s">
         <v>466</v>
       </c>
@@ -13289,7 +13283,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="350" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A350" s="17" t="s">
         <v>467</v>
       </c>
@@ -13303,7 +13297,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="351" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A351" s="17" t="s">
         <v>469</v>
       </c>
@@ -13317,7 +13311,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="352" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A352" s="17" t="s">
         <v>471</v>
       </c>
@@ -13331,7 +13325,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="353" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A353" s="17" t="s">
         <v>473</v>
       </c>
@@ -13345,7 +13339,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="354" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A354" s="17" t="s">
         <v>474</v>
       </c>
@@ -13359,7 +13353,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="355" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A355" s="17" t="s">
         <v>475</v>
       </c>
@@ -13373,7 +13367,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="356" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A356" s="17" t="s">
         <v>477</v>
       </c>
@@ -13387,7 +13381,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="357" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A357" s="17" t="s">
         <v>478</v>
       </c>
@@ -13401,7 +13395,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="358" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A358" s="17" t="s">
         <v>479</v>
       </c>
@@ -13411,7 +13405,7 @@
       </c>
       <c r="E358" s="17"/>
     </row>
-    <row r="359" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A359" s="17" t="s">
         <v>480</v>
       </c>
@@ -13425,7 +13419,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="360" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A360" s="17" t="s">
         <v>481</v>
       </c>
@@ -13435,7 +13429,7 @@
       </c>
       <c r="E360" s="17"/>
     </row>
-    <row r="361" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A361" s="17" t="s">
         <v>482</v>
       </c>
@@ -13445,7 +13439,7 @@
       </c>
       <c r="E361" s="17"/>
     </row>
-    <row r="362" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A362" s="17" t="s">
         <v>483</v>
       </c>
@@ -13459,7 +13453,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="363" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A363" s="17" t="s">
         <v>485</v>
       </c>
@@ -13473,7 +13467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A364" s="17" t="s">
         <v>486</v>
       </c>
@@ -13483,7 +13477,7 @@
       </c>
       <c r="E364" s="17"/>
     </row>
-    <row r="365" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A365" s="17" t="s">
         <v>487</v>
       </c>
@@ -13497,7 +13491,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="366" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A366" s="17" t="s">
         <v>488</v>
       </c>
@@ -13507,7 +13501,7 @@
       </c>
       <c r="E366" s="17"/>
     </row>
-    <row r="367" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A367" s="17" t="s">
         <v>489</v>
       </c>
@@ -13517,7 +13511,7 @@
       </c>
       <c r="E367" s="17"/>
     </row>
-    <row r="368" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A368" s="17" t="s">
         <v>490</v>
       </c>
@@ -13531,7 +13525,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="369" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A369" s="17" t="s">
         <v>491</v>
       </c>
@@ -13545,7 +13539,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="370" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A370" s="17" t="s">
         <v>493</v>
       </c>
@@ -13559,7 +13553,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="371" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A371" s="17" t="s">
         <v>494</v>
       </c>
@@ -13573,7 +13567,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="372" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A372" s="17" t="s">
         <v>495</v>
       </c>
@@ -13583,7 +13577,7 @@
       </c>
       <c r="E372" s="17"/>
     </row>
-    <row r="373" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A373" s="17" t="s">
         <v>496</v>
       </c>
@@ -13597,7 +13591,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="374" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A374" s="17" t="s">
         <v>497</v>
       </c>
@@ -13607,7 +13601,7 @@
       </c>
       <c r="E374" s="17"/>
     </row>
-    <row r="375" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A375" s="17" t="s">
         <v>498</v>
       </c>
@@ -13617,7 +13611,7 @@
       </c>
       <c r="E375" s="17"/>
     </row>
-    <row r="376" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A376" s="17" t="s">
         <v>499</v>
       </c>
@@ -13631,7 +13625,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="377" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A377" s="17" t="s">
         <v>500</v>
       </c>
@@ -13645,7 +13639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A378" s="17" t="s">
         <v>501</v>
       </c>
@@ -13655,7 +13649,7 @@
       </c>
       <c r="E378" s="17"/>
     </row>
-    <row r="379" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A379" s="17" t="s">
         <v>502</v>
       </c>
@@ -13669,7 +13663,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="380" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A380" s="17" t="s">
         <v>503</v>
       </c>
@@ -13679,7 +13673,7 @@
       </c>
       <c r="E380" s="17"/>
     </row>
-    <row r="381" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A381" s="17" t="s">
         <v>504</v>
       </c>
@@ -13689,7 +13683,7 @@
       </c>
       <c r="E381" s="17"/>
     </row>
-    <row r="382" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A382" s="17" t="s">
         <v>505</v>
       </c>
@@ -13703,7 +13697,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="383" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A383" s="17" t="s">
         <v>506</v>
       </c>
@@ -13717,7 +13711,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="384" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A384" s="17" t="s">
         <v>508</v>
       </c>
@@ -13731,7 +13725,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="385" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A385" s="17" t="s">
         <v>509</v>
       </c>
@@ -13745,7 +13739,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="386" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A386" s="17" t="s">
         <v>510</v>
       </c>
@@ -13755,7 +13749,7 @@
       </c>
       <c r="E386" s="17"/>
     </row>
-    <row r="387" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A387" s="17" t="s">
         <v>511</v>
       </c>
@@ -13769,7 +13763,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="388" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A388" s="17" t="s">
         <v>512</v>
       </c>
@@ -13779,7 +13773,7 @@
       </c>
       <c r="E388" s="17"/>
     </row>
-    <row r="389" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A389" s="17" t="s">
         <v>513</v>
       </c>
@@ -13789,7 +13783,7 @@
       </c>
       <c r="E389" s="17"/>
     </row>
-    <row r="390" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A390" s="17" t="s">
         <v>514</v>
       </c>
@@ -13803,7 +13797,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="391" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A391" s="17" t="s">
         <v>515</v>
       </c>
@@ -13817,7 +13811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A392" s="17" t="s">
         <v>516</v>
       </c>
@@ -13827,7 +13821,7 @@
       </c>
       <c r="E392" s="17"/>
     </row>
-    <row r="393" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A393" s="17" t="s">
         <v>517</v>
       </c>
@@ -13841,7 +13835,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="394" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A394" s="17" t="s">
         <v>518</v>
       </c>
@@ -13851,7 +13845,7 @@
       </c>
       <c r="E394" s="17"/>
     </row>
-    <row r="395" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A395" s="17" t="s">
         <v>519</v>
       </c>
@@ -13861,7 +13855,7 @@
       </c>
       <c r="E395" s="17"/>
     </row>
-    <row r="396" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A396" s="17" t="s">
         <v>520</v>
       </c>
@@ -13875,7 +13869,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="397" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A397" s="17" t="s">
         <v>521</v>
       </c>
@@ -13889,7 +13883,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="398" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A398" s="17" t="s">
         <v>523</v>
       </c>
@@ -13903,7 +13897,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="399" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A399" s="17" t="s">
         <v>524</v>
       </c>
@@ -13917,7 +13911,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="400" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A400" s="17" t="s">
         <v>525</v>
       </c>
@@ -13927,7 +13921,7 @@
       </c>
       <c r="E400" s="17"/>
     </row>
-    <row r="401" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A401" s="17" t="s">
         <v>526</v>
       </c>
@@ -13941,7 +13935,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="402" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A402" s="17" t="s">
         <v>527</v>
       </c>
@@ -13951,7 +13945,7 @@
       </c>
       <c r="E402" s="17"/>
     </row>
-    <row r="403" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A403" s="17" t="s">
         <v>528</v>
       </c>
@@ -13961,7 +13955,7 @@
       </c>
       <c r="E403" s="17"/>
     </row>
-    <row r="404" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A404" s="17" t="s">
         <v>529</v>
       </c>
@@ -13975,7 +13969,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="405" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A405" s="17" t="s">
         <v>530</v>
       </c>
@@ -13989,7 +13983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="406" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A406" s="17" t="s">
         <v>531</v>
       </c>
@@ -13999,7 +13993,7 @@
       </c>
       <c r="E406" s="17"/>
     </row>
-    <row r="407" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A407" s="17" t="s">
         <v>532</v>
       </c>
@@ -14013,7 +14007,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="408" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A408" s="17" t="s">
         <v>533</v>
       </c>
@@ -14023,7 +14017,7 @@
       </c>
       <c r="E408" s="17"/>
     </row>
-    <row r="409" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A409" s="17" t="s">
         <v>534</v>
       </c>
@@ -14033,7 +14027,7 @@
       </c>
       <c r="E409" s="17"/>
     </row>
-    <row r="410" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A410" s="17" t="s">
         <v>535</v>
       </c>
@@ -14047,7 +14041,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="411" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A411" s="17" t="s">
         <v>536</v>
       </c>
@@ -14061,7 +14055,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="412" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A412" s="17" t="s">
         <v>538</v>
       </c>
@@ -14075,7 +14069,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="413" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A413" s="17" t="s">
         <v>539</v>
       </c>
@@ -14089,7 +14083,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="414" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A414" s="17" t="s">
         <v>540</v>
       </c>
@@ -14099,7 +14093,7 @@
       </c>
       <c r="E414" s="17"/>
     </row>
-    <row r="415" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A415" s="17" t="s">
         <v>541</v>
       </c>
@@ -14113,7 +14107,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="416" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A416" s="17" t="s">
         <v>542</v>
       </c>
@@ -14123,7 +14117,7 @@
       </c>
       <c r="E416" s="17"/>
     </row>
-    <row r="417" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A417" s="17" t="s">
         <v>543</v>
       </c>
@@ -14133,7 +14127,7 @@
       </c>
       <c r="E417" s="17"/>
     </row>
-    <row r="418" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A418" s="17" t="s">
         <v>544</v>
       </c>
@@ -14147,7 +14141,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="419" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A419" s="17" t="s">
         <v>545</v>
       </c>
@@ -14161,7 +14155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="420" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A420" s="17" t="s">
         <v>546</v>
       </c>
@@ -14175,7 +14169,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="421" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A421" s="17" t="s">
         <v>547</v>
       </c>
@@ -14189,7 +14183,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="422" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A422" s="17" t="s">
         <v>548</v>
       </c>
@@ -14199,7 +14193,7 @@
       </c>
       <c r="E422" s="17"/>
     </row>
-    <row r="423" spans="1:5" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A423" s="17" t="s">
         <v>549</v>
       </c>
@@ -14213,7 +14207,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="424" spans="1:5" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C424" s="23" t="b">
         <v>1</v>
       </c>
@@ -14224,7 +14218,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="425" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C425" s="24" t="b">
         <v>1</v>
       </c>
@@ -14235,7 +14229,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="426" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C426" s="26" t="b">
         <v>1</v>
       </c>
@@ -14246,7 +14240,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="427" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C427" s="26" t="b">
         <v>1</v>
       </c>
@@ -14257,7 +14251,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="428" spans="1:5" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C428" s="26" t="b">
         <v>1</v>
       </c>
@@ -14268,7 +14262,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="429" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C429" s="26" t="b">
         <v>1</v>
       </c>
@@ -14279,7 +14273,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="430" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C430" s="26" t="b">
         <v>1</v>
       </c>
@@ -14290,7 +14284,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="431" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C431" s="26" t="b">
         <v>1</v>
       </c>
@@ -14301,7 +14295,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="432" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C432" s="26" t="b">
         <v>1</v>
       </c>
@@ -14312,7 +14306,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="433" spans="3:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="433" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C433" s="26" t="b">
         <v>1</v>
       </c>
@@ -14323,7 +14317,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="434" spans="3:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="434" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C434" s="26" t="b">
         <v>1</v>
       </c>
@@ -14334,7 +14328,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="435" spans="3:5" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="435" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C435" s="26" t="b">
         <v>1</v>
       </c>
@@ -14345,7 +14339,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="436" spans="3:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="436" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C436" s="26" t="b">
         <v>1</v>
       </c>
@@ -14356,7 +14350,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="437" spans="3:5" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="437" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C437" s="26" t="b">
         <v>1</v>
       </c>
@@ -14367,7 +14361,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="438" spans="3:5" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="438" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C438" s="26" t="b">
         <v>1</v>
       </c>
@@ -14378,7 +14372,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="439" spans="3:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="439" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C439" s="33" t="b">
         <v>1</v>
       </c>
@@ -14389,7 +14383,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="440" spans="3:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="440" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C440" s="33" t="b">
         <v>1</v>
       </c>
@@ -14400,7 +14394,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="441" spans="3:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="441" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C441" s="33" t="b">
         <v>1</v>
       </c>
@@ -14411,7 +14405,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="442" spans="3:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="442" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C442" s="33" t="b">
         <v>1</v>
       </c>
@@ -14422,7 +14416,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="443" spans="3:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="443" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C443" s="33" t="b">
         <v>1</v>
       </c>
@@ -14433,7 +14427,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="444" spans="3:5" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="444" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C444" s="33" t="b">
         <v>1</v>
       </c>
@@ -14444,7 +14438,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="445" spans="3:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="445" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C445" s="33" t="b">
         <v>1</v>
       </c>
@@ -14455,7 +14449,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="446" spans="3:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="446" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C446" s="33" t="b">
         <v>1</v>
       </c>
@@ -14466,7 +14460,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="447" spans="3:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="447" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C447" s="33" t="b">
         <v>1</v>
       </c>
@@ -14477,7 +14471,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="448" spans="3:5" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="448" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C448" s="33" t="b">
         <v>1</v>
       </c>
@@ -14488,7 +14482,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="449" spans="3:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="449" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C449" s="33" t="b">
         <v>1</v>
       </c>
@@ -14499,7 +14493,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="450" spans="3:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="450" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C450" s="33" t="b">
         <v>1</v>
       </c>
@@ -14510,7 +14504,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="451" spans="3:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="451" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C451" s="33" t="b">
         <v>1</v>
       </c>
@@ -14521,7 +14515,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="452" spans="3:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="452" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C452" s="33" t="b">
         <v>1</v>
       </c>
@@ -14532,7 +14526,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="453" spans="3:5" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="453" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C453" s="33" t="b">
         <v>1</v>
       </c>
@@ -14543,7 +14537,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="454" spans="3:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="454" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C454" s="33" t="b">
         <v>1</v>
       </c>
@@ -14554,7 +14548,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="455" spans="3:5" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="455" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C455" s="33" t="b">
         <v>1</v>
       </c>
@@ -14565,7 +14559,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="456" spans="3:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="456" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C456" s="33" t="b">
         <v>1</v>
       </c>
@@ -14576,7 +14570,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="457" spans="3:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="457" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C457" s="33" t="b">
         <v>1</v>
       </c>
@@ -14587,7 +14581,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="458" spans="3:5" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="458" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C458" s="33" t="b">
         <v>1</v>
       </c>
@@ -14598,7 +14592,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="459" spans="3:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="459" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C459" s="26" t="b">
         <v>1</v>
       </c>
@@ -14609,7 +14603,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="460" spans="3:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="460" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C460" s="26" t="b">
         <v>1</v>
       </c>
@@ -14620,7 +14614,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="461" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="461" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C461" s="26" t="b">
         <v>1</v>
       </c>
@@ -14631,7 +14625,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="462" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="462" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C462" s="26" t="b">
         <v>1</v>
       </c>
@@ -14642,7 +14636,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="463" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="463" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C463" s="26" t="b">
         <v>1</v>
       </c>
@@ -14653,7 +14647,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="464" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="464" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C464" s="26" t="b">
         <v>1</v>
       </c>
@@ -14664,7 +14658,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="465" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="465" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C465" s="26" t="b">
         <v>1</v>
       </c>
@@ -14675,7 +14669,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="466" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="466" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C466" s="26" t="b">
         <v>1</v>
       </c>
@@ -14686,7 +14680,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="467" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="467" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C467" s="26" t="b">
         <v>1</v>
       </c>
@@ -14697,7 +14691,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="468" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="468" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C468" s="26" t="b">
         <v>1</v>
       </c>
@@ -14708,7 +14702,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="469" spans="3:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="469" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C469" s="26" t="b">
         <v>1</v>
       </c>
@@ -14719,7 +14713,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="470" spans="3:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="470" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C470" s="26" t="b">
         <v>1</v>
       </c>
@@ -14730,7 +14724,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="471" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="471" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C471" s="26" t="b">
         <v>1</v>
       </c>
@@ -14741,7 +14735,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="472" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="472" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C472" s="26" t="b">
         <v>1</v>
       </c>
@@ -14752,7 +14746,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="473" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="473" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C473" s="26" t="b">
         <v>1</v>
       </c>
@@ -14763,7 +14757,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="474" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="474" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C474" s="26" t="b">
         <v>1</v>
       </c>
@@ -14774,7 +14768,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="475" spans="3:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="475" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C475" s="26" t="b">
         <v>1</v>
       </c>
@@ -14785,7 +14779,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="476" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="476" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C476" s="26" t="b">
         <v>1</v>
       </c>
@@ -14796,7 +14790,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="477" spans="3:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="477" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C477" s="26" t="b">
         <v>1</v>
       </c>
@@ -14807,7 +14801,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="478" spans="3:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="478" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C478" s="26" t="b">
         <v>1</v>
       </c>
@@ -14818,7 +14812,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="479" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="479" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C479" s="26" t="b">
         <v>1</v>
       </c>
@@ -14829,7 +14823,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="480" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="480" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C480" s="26" t="b">
         <v>1</v>
       </c>
@@ -14840,7 +14834,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="481" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="481" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C481" s="26" t="b">
         <v>1</v>
       </c>
@@ -14851,7 +14845,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="482" spans="3:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="482" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C482" s="26" t="b">
         <v>1</v>
       </c>
@@ -14862,7 +14856,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="483" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="483" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C483" s="26" t="b">
         <v>1</v>
       </c>
@@ -14873,7 +14867,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="484" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="484" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C484" s="26" t="b">
         <v>1</v>
       </c>
@@ -14884,7 +14878,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="485" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="485" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C485" s="26" t="b">
         <v>1</v>
       </c>
@@ -14895,7 +14889,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="486" spans="3:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="486" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C486" s="26" t="b">
         <v>1</v>
       </c>
@@ -14906,7 +14900,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="487" spans="3:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="487" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C487" s="26" t="b">
         <v>1</v>
       </c>
@@ -14917,7 +14911,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="488" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="488" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C488" s="26" t="b">
         <v>1</v>
       </c>
@@ -14928,7 +14922,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="489" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="489" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C489" s="26" t="b">
         <v>1</v>
       </c>
@@ -14939,7 +14933,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="490" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="490" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C490" s="26" t="b">
         <v>1</v>
       </c>
@@ -14950,7 +14944,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="491" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="491" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C491" s="26" t="b">
         <v>1</v>
       </c>
@@ -14961,7 +14955,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="492" spans="3:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="492" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C492" s="26" t="b">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
updated .env, commented out update cache in main, added readability spacing to config output text file for missing objs, refactors to match process, added some logging to matcher class, updated user config_structure to include 'src_details':{'tecex-ruleseng:'...}, updated updater
</commit_message>
<xml_diff>
--- a/TestSheet1.xlsx
+++ b/TestSheet1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niravs\Documents\SFCompareAndLoad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F5A481-BF09-440C-986D-C1E48785C4FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B79D2AD-7AEA-409A-AB8C-F51D70EFF105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{BEF77309-A07C-430D-9426-4A4BDF81F07F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28590" activeTab="1" xr2:uid="{BEF77309-A07C-430D-9426-4A4BDF81F07F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2001,7 +2001,7 @@
     <t>Shipment_Order__c.r__Part__c[1].Requirement_Unknown__c</t>
   </si>
   <si>
-    <t>tecex--prod</t>
+    <t>tecex--ruleseng</t>
   </si>
 </sst>
 </file>
@@ -2752,8 +2752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A29EAB9-F893-4E29-8E72-A16D47667C06}">
   <dimension ref="A1:F492"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8867,7 +8867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60E00B09-BA71-4F35-AAD0-572D3DDCA95E}">
   <dimension ref="A1:F492"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>

</xml_diff>